<commit_message>
Updated Traceability Matrix. Working code.
</commit_message>
<xml_diff>
--- a/Docs/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/Docs/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele\Documents\Personal\Continental Automotive Program\Practicas\Michele Window Lifter Working Space\window_lifter_svn\docs\V-Cycle Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele\Documents\Personal\Continental Automotive Program\Practicas\WindowLifter_Sched WS - Michele\Docs\V-Cycle Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2008,9 +2008,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Modifications for MISRA compliance. Code Review document update.
</commit_message>
<xml_diff>
--- a/Docs/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/Docs/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -2008,7 +2008,9 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2408,7 +2410,7 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="C2:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>